<commit_message>
add more manual testing test cases and bug report
</commit_message>
<xml_diff>
--- a/01- Manual-Testing/Bug_Reports.xlsx
+++ b/01- Manual-Testing/Bug_Reports.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\Testing Project\01-Manual-Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\Testing Project\01- Manual-Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20663ED-A9B4-400A-A9BF-4F5465FCFFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777F0864-4D00-4E6B-8AD5-E89B618C39E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Expected Result</t>
   </si>
@@ -128,6 +128,25 @@
     <t>there is an error that when user write the 'lastname' data 
 it is directly moved this data to 'firstname' field 
 and empties the 'lastname' field</t>
+  </si>
+  <si>
+    <t>BUG_004</t>
+  </si>
+  <si>
+    <t>Sorting button not worked</t>
+  </si>
+  <si>
+    <t>1. Navigate to https://www.saucedemo.com
+2. Login with username: error_user
+3. Login with password: secret_sauce
+4. Click Login button
+5.click on sorting button</t>
+  </si>
+  <si>
+    <t>the user must see that the products are sorted as he clicked the sorting choice</t>
+  </si>
+  <si>
+    <t>the user cant sort the products because it shows an error message "sorting is broken"</t>
   </si>
 </sst>
 </file>
@@ -241,21 +260,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Roboto Mono Light"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="0" tint="-0.499984740745262"/>
@@ -502,6 +506,21 @@
           <color theme="0" tint="-0.499984740745262"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Roboto Mono Light"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -538,18 +557,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC6A9F36-130E-4E48-96E3-9F01A773EE3A}" name="Table2" displayName="Table2" ref="A1:I5" totalsRowShown="0" headerRowDxfId="10" dataDxfId="0">
-  <autoFilter ref="A1:I5" xr:uid="{FC6A9F36-130E-4E48-96E3-9F01A773EE3A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FC6A9F36-130E-4E48-96E3-9F01A773EE3A}" name="Table2" displayName="Table2" ref="A1:I11" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I11" xr:uid="{FC6A9F36-130E-4E48-96E3-9F01A773EE3A}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{3230414D-D895-4980-9FC1-8279CA52401E}" name="Bug ID" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{060B1C11-096E-4254-8B64-A8406C8EF1D2}" name="Title" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{6407E56D-1F62-4FCF-B9C2-9BB012A52E5B}" name="Severity" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{C86030FD-B814-4F06-88C4-B793AA823861}" name="Priority" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{D4019C3C-1DAC-48E7-97DC-DA094D343EA5}" name="Steps to Reproduce" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{C30EF743-7DDA-469F-A084-BA52957CAAF1}" name="Expected Result" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{7D85A50F-09EB-457C-9AF4-BA4CCFAD5993}" name="Actual Result" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{805E75DD-572E-444F-8019-D72198AD148E}" name="Status" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{33DDFB41-3EA6-4B8A-A8CE-28D1BCA2478C}" name="Notes \ Attachments" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3230414D-D895-4980-9FC1-8279CA52401E}" name="Bug ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{060B1C11-096E-4254-8B64-A8406C8EF1D2}" name="Title" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{6407E56D-1F62-4FCF-B9C2-9BB012A52E5B}" name="Severity" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{C86030FD-B814-4F06-88C4-B793AA823861}" name="Priority" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{D4019C3C-1DAC-48E7-97DC-DA094D343EA5}" name="Steps to Reproduce" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{C30EF743-7DDA-469F-A084-BA52957CAAF1}" name="Expected Result" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{7D85A50F-09EB-457C-9AF4-BA4CCFAD5993}" name="Actual Result" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{805E75DD-572E-444F-8019-D72198AD148E}" name="Status" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{33DDFB41-3EA6-4B8A-A8CE-28D1BCA2478C}" name="Notes \ Attachments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -820,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,22 +966,98 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
     <row r="12" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -970,7 +1065,7 @@
     <row r="16" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 C2:C5" xr:uid="{9396EB45-17A7-4423-9A6D-E8AD60BEDCCF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5 C2:C11" xr:uid="{9396EB45-17A7-4423-9A6D-E8AD60BEDCCF}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>